<commit_message>
3.4 estratégia de pesquisa
</commit_message>
<xml_diff>
--- a/Projeto2/docs/testes.xlsx
+++ b/Projeto2/docs/testes.xlsx
@@ -232,9 +232,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -263,6 +260,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -6627,13 +6627,13 @@
   <dimension ref="B2:K51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="J8" sqref="B3:J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" customWidth="1"/>
     <col min="4" max="4" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.77734375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25.21875" bestFit="1" customWidth="1"/>
@@ -6644,201 +6644,201 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="13">
+      <c r="C2" s="12">
         <v>10</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="13">
+      <c r="E2" s="12">
         <v>5</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="G2" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B3" s="4"/>
-      <c r="C3" s="11" t="s">
+      <c r="B3" s="14"/>
+      <c r="C3" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="G3" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="H3" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="I3" s="11" t="s">
+      <c r="I3" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="J3" s="11" t="s">
+      <c r="J3" s="10" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="6">
         <v>3.347</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="7">
         <v>1.718</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="6">
         <v>18.071999999999999</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F4" s="6">
         <v>18.707999999999998</v>
       </c>
-      <c r="G4" s="7">
+      <c r="G4" s="6">
         <v>49.706000000000003</v>
       </c>
-      <c r="H4" s="7">
+      <c r="H4" s="6">
         <v>2.8769999999999998</v>
       </c>
-      <c r="I4" s="7">
+      <c r="I4" s="6">
         <v>16.059999999999999</v>
       </c>
-      <c r="J4" s="7">
+      <c r="J4" s="6">
         <v>21.57</v>
       </c>
       <c r="K4" s="3"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="6">
         <v>3.5329999999999999</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="6">
         <v>5.125</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="6">
         <v>18.716999999999999</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="6">
         <v>18.382999999999999</v>
       </c>
-      <c r="G5" s="7">
+      <c r="G5" s="6">
         <v>21.699000000000002</v>
       </c>
-      <c r="H5" s="7">
+      <c r="H5" s="6">
         <v>3.121</v>
       </c>
-      <c r="I5" s="7">
+      <c r="I5" s="6">
         <v>19.539000000000001</v>
       </c>
-      <c r="J5" s="7">
+      <c r="J5" s="6">
         <v>20.85</v>
       </c>
       <c r="K5" s="2"/>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="6">
         <v>3.2229999999999999</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="6">
         <v>2.9969999999999999</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="7">
         <v>73.378</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="6">
         <v>17.606999999999999</v>
       </c>
-      <c r="G6" s="7">
+      <c r="G6" s="6">
         <v>56.771999999999998</v>
       </c>
-      <c r="H6" s="7">
+      <c r="H6" s="6">
         <v>2.9319999999999999</v>
       </c>
-      <c r="I6" s="7">
+      <c r="I6" s="6">
         <v>16.652000000000001</v>
       </c>
-      <c r="J6" s="7">
+      <c r="J6" s="6">
         <v>27.013999999999999</v>
       </c>
       <c r="K6" s="1"/>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="6">
         <v>3.4089999999999998</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="6">
         <v>4.6550000000000002</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E7" s="8">
         <v>28.248999999999999</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="6">
         <v>30.042000000000002</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="6">
         <v>71.760999999999996</v>
       </c>
-      <c r="H7" s="7">
+      <c r="H7" s="6">
         <v>2.9569999999999999</v>
       </c>
-      <c r="I7" s="7">
+      <c r="I7" s="6">
         <v>28.405000000000001</v>
       </c>
-      <c r="J7" s="7">
+      <c r="J7" s="6">
         <v>25.004000000000001</v>
       </c>
       <c r="K7" s="1"/>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="6">
         <v>3.5339999999999998</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="6">
         <v>5.056</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="6">
         <v>28.257000000000001</v>
       </c>
-      <c r="F8" s="7">
+      <c r="F8" s="6">
         <v>23.818000000000001</v>
       </c>
-      <c r="G8" s="7">
+      <c r="G8" s="6">
         <v>69.325000000000003</v>
       </c>
-      <c r="H8" s="7">
+      <c r="H8" s="6">
         <v>3.25</v>
       </c>
-      <c r="I8" s="7">
+      <c r="I8" s="6">
         <v>25.992000000000001</v>
       </c>
-      <c r="J8" s="7">
+      <c r="J8" s="6">
         <v>25.295000000000002</v>
       </c>
       <c r="K8" s="1"/>
@@ -6854,347 +6854,347 @@
       <c r="J9" s="1"/>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="14">
+      <c r="C11" s="13">
         <v>3</v>
       </c>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="D12" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="11" t="s">
+      <c r="E12" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F12" s="11" t="s">
+      <c r="F12" s="10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B13" s="11">
+      <c r="B13" s="10">
         <v>3</v>
       </c>
-      <c r="C13" s="9">
+      <c r="C13" s="8">
         <v>2E-3</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="4">
         <v>2</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13" s="4">
         <v>78</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="F13" s="4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B14" s="11">
+      <c r="B14" s="10">
         <v>5</v>
       </c>
-      <c r="C14" s="9">
+      <c r="C14" s="8">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="4">
         <v>20</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E14" s="4">
         <v>186</v>
       </c>
-      <c r="F14" s="5" t="s">
+      <c r="F14" s="4" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B15" s="11">
+      <c r="B15" s="10">
         <v>7</v>
       </c>
-      <c r="C15" s="9">
+      <c r="C15" s="8">
         <v>2.9000000000000001E-2</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" s="4">
         <v>148</v>
       </c>
-      <c r="E15" s="5">
+      <c r="E15" s="4">
         <v>342</v>
       </c>
-      <c r="F15" s="5" t="s">
+      <c r="F15" s="4" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B16" s="11">
+      <c r="B16" s="10">
         <v>9</v>
       </c>
-      <c r="C16" s="9">
+      <c r="C16" s="8">
         <v>0.11799999999999999</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D16" s="4">
         <v>512</v>
       </c>
-      <c r="E16" s="5">
+      <c r="E16" s="4">
         <v>546</v>
       </c>
-      <c r="F16" s="5" t="s">
+      <c r="F16" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B17" s="11">
+      <c r="B17" s="10">
         <v>11</v>
       </c>
-      <c r="C17" s="9">
+      <c r="C17" s="8">
         <v>0.497</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D17" s="4">
         <v>2869</v>
       </c>
-      <c r="E17" s="5">
+      <c r="E17" s="4">
         <v>798</v>
       </c>
-      <c r="F17" s="5" t="s">
+      <c r="F17" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B18" s="11">
+      <c r="B18" s="10">
         <v>13</v>
       </c>
-      <c r="C18" s="9">
+      <c r="C18" s="8">
         <v>6.08</v>
       </c>
-      <c r="D18" s="5">
+      <c r="D18" s="4">
         <v>54511</v>
       </c>
-      <c r="E18" s="5">
+      <c r="E18" s="4">
         <v>1098</v>
       </c>
-      <c r="F18" s="10" t="s">
+      <c r="F18" s="9" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B19" s="11">
+      <c r="B19" s="10">
         <v>15</v>
       </c>
-      <c r="C19" s="9">
+      <c r="C19" s="8">
         <v>24.4</v>
       </c>
-      <c r="D19" s="5">
+      <c r="D19" s="4">
         <v>311614</v>
       </c>
-      <c r="E19" s="5">
+      <c r="E19" s="4">
         <v>1446</v>
       </c>
-      <c r="F19" s="10" t="s">
+      <c r="F19" s="9" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B40" s="11" t="s">
+      <c r="B40" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C40" s="14">
+      <c r="C40" s="13">
         <v>10</v>
       </c>
-      <c r="D40" s="6"/>
-      <c r="E40" s="6"/>
-      <c r="F40" s="6"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="5"/>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B41" s="11" t="s">
+      <c r="B41" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C41" s="11" t="s">
+      <c r="C41" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D41" s="11" t="s">
+      <c r="D41" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E41" s="11" t="s">
+      <c r="E41" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F41" s="11" t="s">
+      <c r="F41" s="10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B42" s="11">
+      <c r="B42" s="10">
         <v>1</v>
       </c>
-      <c r="C42" s="7">
+      <c r="C42" s="6">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="D42" s="5">
+      <c r="D42" s="4">
         <v>9</v>
       </c>
-      <c r="E42" s="5">
+      <c r="E42" s="4">
         <v>468</v>
       </c>
-      <c r="F42" s="10" t="s">
+      <c r="F42" s="9" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B43" s="11">
+      <c r="B43" s="10">
         <v>2</v>
       </c>
-      <c r="C43" s="7">
+      <c r="C43" s="6">
         <v>0.192</v>
       </c>
-      <c r="D43" s="5">
+      <c r="D43" s="4">
         <v>1300</v>
       </c>
-      <c r="E43" s="5">
+      <c r="E43" s="4">
         <v>666</v>
       </c>
-      <c r="F43" s="10" t="s">
+      <c r="F43" s="9" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B44" s="11">
+      <c r="B44" s="10">
         <v>3</v>
       </c>
-      <c r="C44" s="7">
+      <c r="C44" s="6">
         <v>0.26400000000000001</v>
       </c>
-      <c r="D44" s="5">
+      <c r="D44" s="4">
         <v>1723</v>
       </c>
-      <c r="E44" s="5">
+      <c r="E44" s="4">
         <v>666</v>
       </c>
-      <c r="F44" s="10" t="s">
+      <c r="F44" s="9" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="45" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B45" s="11">
+      <c r="B45" s="10">
         <v>4</v>
       </c>
-      <c r="C45" s="7">
+      <c r="C45" s="6">
         <v>0.57999999999999996</v>
       </c>
-      <c r="D45" s="5">
+      <c r="D45" s="4">
         <v>2696</v>
       </c>
-      <c r="E45" s="5">
+      <c r="E45" s="4">
         <v>666</v>
       </c>
-      <c r="F45" s="10" t="s">
+      <c r="F45" s="9" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="46" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B46" s="11">
+      <c r="B46" s="10">
         <v>5</v>
       </c>
-      <c r="C46" s="7">
+      <c r="C46" s="6">
         <v>1.6180000000000001</v>
       </c>
-      <c r="D46" s="5">
+      <c r="D46" s="4">
         <v>8693</v>
       </c>
-      <c r="E46" s="5">
+      <c r="E46" s="4">
         <v>666</v>
       </c>
-      <c r="F46" s="10" t="s">
+      <c r="F46" s="9" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="47" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B47" s="11">
+      <c r="B47" s="10">
         <v>6</v>
       </c>
-      <c r="C47" s="7">
+      <c r="C47" s="6">
         <v>0.91800000000000004</v>
       </c>
-      <c r="D47" s="5">
+      <c r="D47" s="4">
         <v>4839</v>
       </c>
-      <c r="E47" s="5">
+      <c r="E47" s="4">
         <v>666</v>
       </c>
-      <c r="F47" s="10" t="s">
+      <c r="F47" s="9" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="48" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B48" s="11">
+      <c r="B48" s="10">
         <v>7</v>
       </c>
-      <c r="C48" s="7">
+      <c r="C48" s="6">
         <v>1.087</v>
       </c>
-      <c r="D48" s="5">
+      <c r="D48" s="4">
         <v>5406</v>
       </c>
-      <c r="E48" s="5">
+      <c r="E48" s="4">
         <v>666</v>
       </c>
-      <c r="F48" s="10" t="s">
+      <c r="F48" s="9" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="49" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B49" s="11">
+      <c r="B49" s="10">
         <v>8</v>
       </c>
-      <c r="C49" s="7">
+      <c r="C49" s="6">
         <v>0.35199999999999998</v>
       </c>
-      <c r="D49" s="5">
+      <c r="D49" s="4">
         <v>1527</v>
       </c>
-      <c r="E49" s="5">
+      <c r="E49" s="4">
         <v>666</v>
       </c>
-      <c r="F49" s="10" t="s">
+      <c r="F49" s="9" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="50" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B50" s="11">
+      <c r="B50" s="10">
         <v>9</v>
       </c>
-      <c r="C50" s="7">
+      <c r="C50" s="6">
         <v>0.78600000000000003</v>
       </c>
-      <c r="D50" s="5">
+      <c r="D50" s="4">
         <v>4710</v>
       </c>
-      <c r="E50" s="5">
+      <c r="E50" s="4">
         <v>666</v>
       </c>
-      <c r="F50" s="10" t="s">
+      <c r="F50" s="9" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="51" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B51" s="11">
+      <c r="B51" s="10">
         <v>10</v>
       </c>
-      <c r="C51" s="7">
+      <c r="C51" s="6">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="D51" s="5">
+      <c r="D51" s="4">
         <v>9</v>
       </c>
-      <c r="E51" s="5">
+      <c r="E51" s="4">
         <v>666</v>
       </c>
-      <c r="F51" s="10" t="s">
+      <c r="F51" s="9" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>